<commit_message>
Updates to indicator metadata
</commit_message>
<xml_diff>
--- a/Data/Lagged Indicator Metadata.xlsx
+++ b/Data/Lagged Indicator Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11856"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Indicator Name</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Los of sea ice likely decreases both food quality and quantity supplied to the benthos for early juveniles</t>
+  </si>
+  <si>
+    <t>juv_condition</t>
+  </si>
+  <si>
+    <t>Males collected for this indicator are larger than 50-65mm, but lag 0 assuming similar mechanism between cohorts for reduced condition within a year</t>
   </si>
 </sst>
 </file>
@@ -476,21 +482,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="79" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +514,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -522,7 +528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -536,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -550,7 +556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -564,7 +570,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -572,13 +578,13 @@
         <v>23</v>
       </c>
       <c r="C6" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -592,7 +598,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -606,7 +612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -620,7 +626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -634,7 +640,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -648,7 +654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -662,35 +668,49 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final touches to BAS and figures
</commit_message>
<xml_diff>
--- a/Data/Lagged Indicator Metadata.xlsx
+++ b/Data/Lagged Indicator Metadata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Indicator Name</t>
   </si>
@@ -80,12 +80,6 @@
     <t>Chla</t>
   </si>
   <si>
-    <t>Indicator timeseries too short, removed from BAS suite of indicators</t>
-  </si>
-  <si>
-    <t>Represents prey items across ontogeny</t>
-  </si>
-  <si>
     <t>Rationale for assigning lag</t>
   </si>
   <si>
@@ -95,12 +89,6 @@
     <t>Hypothesized to affect larval stages (Szuwalski et al 2021)</t>
   </si>
   <si>
-    <t>Prevelance highest in small, immature crab</t>
-  </si>
-  <si>
-    <t>Juvenile snow crab habitat</t>
-  </si>
-  <si>
     <t xml:space="preserve">Most cod predation happens at 10-20mm (cod stomach data) </t>
   </si>
   <si>
@@ -110,19 +98,31 @@
     <t>Model Lag (in years)</t>
   </si>
   <si>
-    <t>Recruitment output from 2021 approved model. 2020 data is missing b/c the status quo model does not report the last year of recruitment because it's not considered reliable. Size crab recruiting to the model are 35-45mm carapace width, and therefore likely 4-5 years post-settlement)</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>Los of sea ice likely decreases both food quality and quantity supplied to the benthos for early juveniles</t>
-  </si>
-  <si>
     <t>juv_condition</t>
   </si>
   <si>
-    <t>Males collected for this indicator are larger than 50-65mm, but lag 0 assuming similar mechanism between cohorts for reduced condition within a year</t>
+    <t>Diatoms are a key prey item for larval stages</t>
+  </si>
+  <si>
+    <t>Recruitment output from 2022 approved model. Note that the final few years of recruitment estimates are fairly unreliable. Size crab recruiting to the model are 25-40mm carapace width, and therefore likely 3-4 years post-settlement</t>
+  </si>
+  <si>
+    <t>Los of sea ice likely decreases both food quality and quantity supplied to the benthos for early juveniles- Copeman et. al research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Represents prey items across ontogeny. Missing polychetes, which are preferential juvenile crab prey. Limited prey may influence survival to recruitment the following year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juvenile snow crab habitat; high temperatures may indirectly or directly affect survival to recruitment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Males collected for this indicator are larger than 50-65mm, assuming similar mechanism between cohorts for reduced condition within a year. Poor condition suggests poor survival to recruitment the following year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Highest prevelances are in small juveniles- affecting survival to recruitment  </t>
   </si>
 </sst>
 </file>
@@ -485,13 +485,13 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="79" customWidth="1"/>
+    <col min="2" max="2" width="84.109375" customWidth="1"/>
     <col min="3" max="3" width="23.5546875" customWidth="1"/>
     <col min="4" max="4" width="21.109375" customWidth="1"/>
   </cols>
@@ -501,13 +501,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
@@ -519,13 +519,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -533,10 +533,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="6">
         <v>2</v>
@@ -547,13 +547,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -564,10 +564,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -575,10 +575,10 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C6" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -592,10 +592,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -603,13 +603,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -617,13 +617,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="6">
         <v>3</v>
       </c>
       <c r="D9" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -634,10 +634,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -645,13 +645,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="6">
         <v>3</v>
       </c>
       <c r="D11" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -659,27 +659,27 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
       <c r="C13" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -703,7 +703,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>